<commit_message>
legado: PMQA - PONTOS
</commit_message>
<xml_diff>
--- a/public/file/Servico/PMQA/Ponto/modelo_planilha_pontos_pmqa_teste.xlsx
+++ b/public/file/Servico/PMQA/Ponto/modelo_planilha_pontos_pmqa_teste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DNIT\ECOSistemas DNIT - 50600.0019502021-01 - 9399\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Marcos\ecossistema-v2\public\file\Servico\PMQA\Ponto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A8167ED-F20E-414C-9179-45198BA76211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B651C28-C5B7-4973-AA45-5C91417F7187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
-    <t>NomePontoColeta</t>
-  </si>
-  <si>
     <t>Lat_x</t>
   </si>
   <si>
@@ -42,18 +39,12 @@
     <t>Classe</t>
   </si>
   <si>
-    <t>TipoAmbiente</t>
-  </si>
-  <si>
     <t>UF</t>
   </si>
   <si>
     <t>Municipio</t>
   </si>
   <si>
-    <t>BaciaHidrografica</t>
-  </si>
-  <si>
     <t>Km_rodovia</t>
   </si>
   <si>
@@ -103,6 +94,15 @@
   </si>
   <si>
     <t>Rio das Almas</t>
+  </si>
+  <si>
+    <t>nome_ponto_coleta</t>
+  </si>
+  <si>
+    <t>bacia_hidrografica</t>
+  </si>
+  <si>
+    <t>Tipo_ambiente</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,45 +565,45 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2">
         <v>-9.7009690000000006</v>
@@ -612,22 +612,22 @@
         <v>-41.513024000000001</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
       </c>
       <c r="J2">
         <v>15</v>
@@ -636,12 +636,12 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2">
         <v>-9.6892200000000006</v>
@@ -650,22 +650,22 @@
         <v>-41.375605999999998</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J3">
         <v>25</v>
@@ -674,12 +674,12 @@
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2">
         <v>-9.7179149999999996</v>
@@ -688,22 +688,22 @@
         <v>-41.650658999999997</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
         <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
       </c>
       <c r="J4">
         <v>35</v>
@@ -712,12 +712,12 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2">
         <v>-9.7838989999999999</v>
@@ -726,22 +726,22 @@
         <v>-41.660938000000002</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J5">
         <v>45</v>
@@ -750,12 +750,12 @@
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2">
         <v>-9.6877230000000001</v>
@@ -764,22 +764,22 @@
         <v>-41.679609999999997</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
         <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" t="s">
-        <v>17</v>
       </c>
       <c r="J6">
         <v>55</v>
@@ -788,12 +788,12 @@
         <v>5</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2">
         <v>-9.6382539999999999</v>
@@ -802,22 +802,22 @@
         <v>-41.257781000000001</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J7">
         <v>65</v>
@@ -826,7 +826,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>